<commit_message>
Master -- add new formulas and change functions - Trade
</commit_message>
<xml_diff>
--- a/data/input/Book1.xlsx
+++ b/data/input/Book1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisareade/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/DEVELOPMENT/FREELANCER/excelWeb_script/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F070B1BC-37C1-BD46-94F0-F4A58460FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5592666D-CD95-4448-996F-8875B7BA73BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16660" xr2:uid="{D88A5C88-6097-7E42-8EE0-42D525BBE7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,19 +62,19 @@
     <t>JBLU Mar 15 2024 4.0 Put</t>
   </si>
   <si>
+    <t>WBD Feb 16 2024 10.0 Put</t>
+  </si>
+  <si>
+    <t>Sold to Open 1 BABA Feb 16 2024 70.0 Put @ 2.07</t>
+  </si>
+  <si>
+    <t>BABA Feb 16 2024 70.0 Put</t>
+  </si>
+  <si>
+    <t>***END OF FILE***</t>
+  </si>
+  <si>
     <t>Sold to Open 4 WBD Feb 16 2024 10.0 Put @ 0.24</t>
-  </si>
-  <si>
-    <t>WBD Feb 16 2024 10.0 Put</t>
-  </si>
-  <si>
-    <t>Sold to Open 1 BABA Feb 16 2024 70.0 Put @ 2.07</t>
-  </si>
-  <si>
-    <t>BABA Feb 16 2024 70.0 Put</t>
-  </si>
-  <si>
-    <t>***END OF FILE***</t>
   </si>
 </sst>
 </file>
@@ -153,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,12 +452,12 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="85.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -518,13 +518,13 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4">
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4">
         <v>0.24</v>
@@ -544,13 +544,13 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4">
         <v>2.0699999999999998</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>

</xml_diff>